<commit_message>
Tipo de datos corregidos
</commit_message>
<xml_diff>
--- a/Descripcion inicial.xlsx
+++ b/Descripcion inicial.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dakurei\Desktop\Descriptiva-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NICO\Desktop\TG#2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A6B523-6AC4-4DB4-960D-945FC58A28A5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{380C8AA8-68F8-4CE8-A642-0F0C758EF4D2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>Variables por persona</t>
   </si>
@@ -36,21 +35,12 @@
     <t>ESTCIVIL</t>
   </si>
   <si>
-    <t>CONYUVIVE</t>
-  </si>
-  <si>
-    <t>HIJOSDE</t>
-  </si>
-  <si>
     <t>SEXO</t>
   </si>
   <si>
     <t>EMBARAZA</t>
   </si>
   <si>
-    <t>FECHANTO</t>
-  </si>
-  <si>
     <t>DISCAPA</t>
   </si>
   <si>
@@ -126,9 +116,6 @@
     <t>TCUARTOSVI</t>
   </si>
   <si>
-    <t>THOGAR</t>
-  </si>
-  <si>
     <t>TIPODOC</t>
   </si>
   <si>
@@ -247,12 +234,15 @@
   </si>
   <si>
     <t>Variables por hogar</t>
+  </si>
+  <si>
+    <t>EDAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -688,11 +678,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22DE10E9-B284-4298-98C0-6C5367FBAAD4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,16 +698,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -726,7 +716,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -735,297 +725,291 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="9"/>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>7</v>
+      <c r="A9" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>15</v>
+      <c r="A17" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>17</v>
+      <c r="A19" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D25" s="7"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>